<commit_message>
make current volume optional
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_QC_v4_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_QC_v4_8_0.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="448">
   <si>
     <t xml:space="preserve">Sample QC Template</t>
   </si>
@@ -2099,10 +2099,10 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2162,9 +2162,7 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
         <v>3</v>
@@ -25170,7 +25168,7 @@
   </sheetPr>
   <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -26094,7 +26092,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>